<commit_message>
try at home now
</commit_message>
<xml_diff>
--- a/testtestresults.xlsx
+++ b/testtestresults.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pythonandsublime\Github_repo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>Skus</t>
   </si>
@@ -99,6 +94,9 @@
     <t>088522500611</t>
   </si>
   <si>
+    <t>2 listings found (excluding us). Price set to .3*First + .7*Second</t>
+  </si>
+  <si>
     <t>10 listings (listing price = 48.28)</t>
   </si>
   <si>
@@ -109,9 +107,6 @@
   </si>
   <si>
     <t>612959900234</t>
-  </si>
-  <si>
-    <t>2 listings found (excluding us). Price set to .3*First + .7*Second</t>
   </si>
   <si>
     <t>3 listings (list price = 239.86)</t>
@@ -123,19 +118,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -151,25 +147,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -435,26 +422,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="67.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="67.85546875"/>
+    <col customWidth="1" max="2" min="2" width="18.5703125"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" width="10"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="14.7109375"/>
+    <col customWidth="1" max="6" min="6" width="12.28515625"/>
+    <col customWidth="1" max="7" min="7" width="11.42578125"/>
+    <col customWidth="1" max="8" min="8" width="9.85546875"/>
+    <col customWidth="1" max="9" min="9" width="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,330 +477,330 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>175.96</v>
       </c>
       <c r="D2">
-        <f>0.9*C2-E2-14.71</f>
-        <v>23.893999999999998</v>
-      </c>
-      <c r="E2">
+        <f>.9*C2-E2-14.71</f>
+        <v/>
+      </c>
+      <c r="E2" t="n">
         <v>119.76</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="n">
         <v>9</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="n">
         <v>11</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="n">
         <v>13</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="n">
         <v>38</v>
       </c>
       <c r="J2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>201.13</v>
       </c>
       <c r="D3">
-        <f>0.9*C3-E3-14.71</f>
-        <v>46.54699999999999</v>
-      </c>
-      <c r="E3">
+        <f>.9*C3-E3-14.71</f>
+        <v/>
+      </c>
+      <c r="E3" t="n">
         <v>119.76</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="n">
         <v>9</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="n">
         <v>11</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="n">
         <v>13</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="n">
         <v>38</v>
       </c>
       <c r="J3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>221.3</v>
       </c>
       <c r="D4">
-        <f>0.9*C4-E4-14.71</f>
-        <v>64.700000000000017</v>
-      </c>
-      <c r="E4">
+        <f>.9*C4-E4-14.71</f>
+        <v/>
+      </c>
+      <c r="E4" t="n">
         <v>119.76</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="n">
         <v>9</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="n">
         <v>11</v>
       </c>
-      <c r="H4">
+      <c r="H4" t="n">
         <v>13</v>
       </c>
-      <c r="I4">
+      <c r="I4" t="n">
         <v>38</v>
       </c>
       <c r="J4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5">
-        <v>249.46</v>
+      <c r="C5" t="n">
+        <v>293.78</v>
       </c>
       <c r="D5">
-        <f>0.9*C5-E5-23.83</f>
-        <v>2.2340000000000231</v>
-      </c>
-      <c r="E5">
+        <f>.9*C5-E5-23.83</f>
+        <v/>
+      </c>
+      <c r="E5" t="n">
         <v>198.45</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="n">
         <v>10.55</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="n">
         <v>10</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="n">
         <v>21</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="n">
         <v>44</v>
       </c>
       <c r="J5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="C6">
-        <v>221.24</v>
+      <c r="C6" t="n">
+        <v>299.49</v>
       </c>
       <c r="D6">
-        <f>0.9*C6-E6-23.83</f>
-        <v>-23.163999999999973</v>
-      </c>
-      <c r="E6">
+        <f>.9*C6-E6-23.83</f>
+        <v/>
+      </c>
+      <c r="E6" t="n">
         <v>198.45</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="n">
         <v>9.9</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="n">
         <v>10</v>
       </c>
-      <c r="H6">
+      <c r="H6" t="n">
         <v>21</v>
       </c>
-      <c r="I6">
+      <c r="I6" t="n">
         <v>44</v>
       </c>
       <c r="J6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="n">
         <v>46.62</v>
       </c>
       <c r="D7">
-        <f>0.9*C7-E7-5.3</f>
-        <v>5.5379999999999976</v>
-      </c>
-      <c r="E7">
+        <f>.9*C7-E7-5.3</f>
+        <v/>
+      </c>
+      <c r="E7" t="n">
         <v>31.12</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="n">
         <v>1.2</v>
       </c>
-      <c r="G7">
+      <c r="G7" t="n">
         <v>3</v>
       </c>
-      <c r="H7">
+      <c r="H7" t="n">
         <v>7</v>
       </c>
-      <c r="I7">
+      <c r="I7" t="n">
         <v>41</v>
       </c>
       <c r="J7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="C8">
-        <v>36.29</v>
+      <c r="C8" t="n">
+        <v>51.24</v>
       </c>
       <c r="D8">
-        <f>0.9*C8-E8-5.3</f>
-        <v>-3.7589999999999995</v>
-      </c>
-      <c r="E8">
+        <f>.9*C8-E8-5.3</f>
+        <v/>
+      </c>
+      <c r="E8" t="n">
         <v>31.12</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="n">
         <v>1.5</v>
       </c>
-      <c r="G8">
+      <c r="G8" t="n">
         <v>3</v>
       </c>
-      <c r="H8">
+      <c r="H8" t="n">
         <v>7</v>
       </c>
-      <c r="I8">
+      <c r="I8" t="n">
         <v>41</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9">
-        <v>48.28</v>
+        <v>28</v>
+      </c>
+      <c r="C9" t="n">
+        <v>52.56</v>
       </c>
       <c r="D9">
-        <f>0.9*C9-E9-5.3</f>
-        <v>7.0320000000000045</v>
-      </c>
-      <c r="E9">
+        <f>.9*C9-E9-5.3</f>
+        <v/>
+      </c>
+      <c r="E9" t="n">
         <v>31.12</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="n">
         <v>1.4</v>
       </c>
-      <c r="G9">
+      <c r="G9" t="n">
         <v>3</v>
       </c>
-      <c r="H9">
+      <c r="H9" t="n">
         <v>7</v>
       </c>
-      <c r="I9">
+      <c r="I9" t="n">
         <v>41</v>
       </c>
       <c r="J9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10">
+        <v>30</v>
+      </c>
+      <c r="C10" t="n">
         <v>257.08</v>
       </c>
       <c r="D10">
-        <f>0.9*C10-E10-14.71</f>
-        <v>60.771999999999998</v>
-      </c>
-      <c r="E10">
-        <v>155.88999999999999</v>
-      </c>
-      <c r="F10">
+        <f>.9*C10-E10-14.71</f>
+        <v/>
+      </c>
+      <c r="E10" t="n">
+        <v>155.89</v>
+      </c>
+      <c r="F10" t="n">
         <v>12</v>
       </c>
-      <c r="G10">
+      <c r="G10" t="n">
         <v>11</v>
       </c>
-      <c r="H10">
+      <c r="H10" t="n">
         <v>13</v>
       </c>
-      <c r="I10">
+      <c r="I10" t="n">
         <v>38</v>
       </c>
       <c r="J10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="n">
         <v>239.86</v>
       </c>
       <c r="D11">
-        <f>0.9*C11-E11-14.71</f>
-        <v>45.274000000000036</v>
-      </c>
-      <c r="E11">
-        <v>155.88999999999999</v>
-      </c>
-      <c r="F11">
+        <f>.9*C11-E11-14.71</f>
+        <v/>
+      </c>
+      <c r="E11" t="n">
+        <v>155.89</v>
+      </c>
+      <c r="F11" t="n">
         <v>12</v>
       </c>
-      <c r="G11">
+      <c r="G11" t="n">
         <v>11</v>
       </c>
-      <c r="H11">
+      <c r="H11" t="n">
         <v>13</v>
       </c>
-      <c r="I11">
+      <c r="I11" t="n">
         <v>38</v>
       </c>
       <c r="J11" t="s">
@@ -817,6 +808,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>